<commit_message>
Incident View Form Test
</commit_message>
<xml_diff>
--- a/doc/Variables.xlsx
+++ b/doc/Variables.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ad551938fa2b33e/Dokumente/GitHub/digibp-saentis/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelschmid/Documents/_Education/FHNW/_DOBP/digibp-saentis/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{DC58EF74-A299-460A-B246-20A79BC03A79}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{7A7A3AA6-7B65-48CD-82E8-104D3EBDB9E0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6465" xr2:uid="{A8A6DDCB-7493-457F-8A5D-1D270983E3E9}"/>
+    <workbookView xWindow="9300" yWindow="460" windowWidth="16180" windowHeight="13600"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Variable</t>
   </si>
@@ -160,11 +159,20 @@
 WEBFORM
 EMAIL</t>
   </si>
+  <si>
+    <t>isReallyIncident</t>
+  </si>
+  <si>
+    <t>Is this really an Incident?</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,7 +233,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -241,7 +249,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -536,22 +544,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8B7E91-E28C-499E-9CE8-5F1B310864A1}">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="2"/>
+    <col min="5" max="5" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -568,7 +576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -582,7 +590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -596,7 +604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -610,7 +618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -624,7 +632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -638,7 +646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -655,7 +663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -669,7 +677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -683,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -697,7 +705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -714,7 +722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -728,7 +736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -742,7 +750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -756,7 +764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -767,6 +775,20 @@
         <v>40</v>
       </c>
       <c r="D15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add incident support gateway
</commit_message>
<xml_diff>
--- a/doc/Variables.xlsx
+++ b/doc/Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="460" windowWidth="16180" windowHeight="13600"/>
+    <workbookView xWindow="3980" yWindow="460" windowWidth="16180" windowHeight="13600"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Variable</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Summary</t>
-  </si>
-  <si>
-    <t>SystemID</t>
   </si>
   <si>
     <t>System ID</t>
@@ -167,6 +164,15 @@
   </si>
   <si>
     <t>Boolean</t>
+  </si>
+  <si>
+    <t>systemID</t>
+  </si>
+  <si>
+    <t>incidentSupported</t>
+  </si>
+  <si>
+    <t>Is this incident supported?</t>
   </si>
 </sst>
 </file>
@@ -545,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -573,7 +579,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.2">
@@ -584,7 +590,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -598,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -612,7 +618,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -648,10 +654,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -660,15 +666,15 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -679,10 +685,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -693,10 +699,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -707,10 +713,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
@@ -719,15 +725,15 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -738,13 +744,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -752,13 +758,13 @@
     </row>
     <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -766,13 +772,13 @@
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -780,15 +786,29 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>